<commit_message>
Version 2 - Updated programme with updating the Ui.path system activities and Ui.Automation activties to an older verison, version 22.4.5
</commit_message>
<xml_diff>
--- a/Supporting Files/Config.xlsx
+++ b/Supporting Files/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janderson141\Desktop\Timesheet - V2 - Digital Asset Lab\Supporting Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janderson141\Documents\Deployed Automations\Timesheet - V2 - Digital Asset Lab\Supporting Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08F71E5-DACB-4B2E-95EB-AC097AE226DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEF17CE-0BAE-403B-97CC-20760BA13667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{1178CC5A-9A94-4B2B-809F-D0239E1C13C7}"/>
   </bookViews>
@@ -140,16 +140,16 @@
     <t>TimChargeAttachBrowser</t>
   </si>
   <si>
+    <t>TimeChargeTableRow</t>
+  </si>
+  <si>
     <t>Input\Customised Time Charge.xlsx</t>
   </si>
   <si>
-    <t>Output\Screen shot</t>
-  </si>
-  <si>
-    <t>Output\Run time execution confirmation</t>
-  </si>
-  <si>
-    <t>TimeChargeTableRow</t>
+    <t xml:space="preserve">Output\Screen shot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output\Run time execution confirmation </t>
   </si>
 </sst>
 </file>
@@ -593,7 +593,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,20 +614,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -635,20 +635,20 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -656,20 +656,20 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -690,7 +690,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>

</xml_diff>